<commit_message>
Behaviors and attitude queries updated
</commit_message>
<xml_diff>
--- a/Resources/Compiled.xlsx
+++ b/Resources/Compiled.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tyleah1/Desktop/nyc_squirrels/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A0010D0C-9D03-8743-98C4-5A0A747B44A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{591D1D2A-67C9-FB4B-AC22-50D25162F1F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16960" xr2:uid="{2CC0A3FC-6AB6-1249-9AAB-1F178B143B2D}"/>
+    <workbookView xWindow="3760" yWindow="460" windowWidth="21720" windowHeight="16960" xr2:uid="{2CC0A3FC-6AB6-1249-9AAB-1F178B143B2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,9 +34,141 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="39">
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>running</t>
+  </si>
+  <si>
+    <t>chasing</t>
+  </si>
+  <si>
+    <t>climbing</t>
+  </si>
+  <si>
+    <t>eating</t>
+  </si>
+  <si>
+    <t>foraging</t>
+  </si>
+  <si>
+    <t>kuks</t>
+  </si>
+  <si>
+    <t>quaas</t>
+  </si>
+  <si>
+    <t>moans</t>
+  </si>
+  <si>
+    <t>tail_flags</t>
+  </si>
+  <si>
+    <t>tail_twitches</t>
+  </si>
+  <si>
+    <t>approaches</t>
+  </si>
+  <si>
+    <t>indifferent</t>
+  </si>
+  <si>
+    <t>runs_from</t>
+  </si>
+  <si>
+    <t>fur_color</t>
+  </si>
+  <si>
+    <t>above</t>
+  </si>
+  <si>
+    <t>ground</t>
+  </si>
+  <si>
+    <t>Adult</t>
+  </si>
+  <si>
+    <t>Juvenile</t>
+  </si>
+  <si>
+    <t>Black</t>
+  </si>
+  <si>
+    <t>Cinammon</t>
+  </si>
+  <si>
+    <t>Gray</t>
+  </si>
+  <si>
+    <t>approaches %</t>
+  </si>
+  <si>
+    <t>indifferent %</t>
+  </si>
+  <si>
+    <t>runs_from %</t>
+  </si>
+  <si>
+    <t>above %</t>
+  </si>
+  <si>
+    <t>ground %</t>
+  </si>
+  <si>
+    <t>running %</t>
+  </si>
+  <si>
+    <t>chasing %</t>
+  </si>
+  <si>
+    <t>climbing %</t>
+  </si>
+  <si>
+    <t>eating %</t>
+  </si>
+  <si>
+    <t>foraging %</t>
+  </si>
+  <si>
+    <t>kuks %</t>
+  </si>
+  <si>
+    <t>quaas %</t>
+  </si>
+  <si>
+    <t>moans %</t>
+  </si>
+  <si>
+    <t>tail_flags %</t>
+  </si>
+  <si>
+    <t>tail_twitches %</t>
+  </si>
+  <si>
+    <t>Totals</t>
+  </si>
+  <si>
+    <t>Total_age</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="0.0%"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -62,14 +194,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -381,12 +516,657 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99D8C755-B0EB-9540-A1B2-9FD485A6C973}">
-  <dimension ref="A1"/>
+  <dimension ref="B1:AI7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="2:35" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O1" t="s">
+        <v>5</v>
+      </c>
+      <c r="P1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>7</v>
+      </c>
+      <c r="R1" t="s">
+        <v>8</v>
+      </c>
+      <c r="S1" t="s">
+        <v>9</v>
+      </c>
+      <c r="T1" t="s">
+        <v>10</v>
+      </c>
+      <c r="U1" t="s">
+        <v>22</v>
+      </c>
+      <c r="V1" t="s">
+        <v>23</v>
+      </c>
+      <c r="W1" t="s">
+        <v>24</v>
+      </c>
+      <c r="X1" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="2:35" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2">
+        <v>92</v>
+      </c>
+      <c r="E2">
+        <v>100</v>
+      </c>
+      <c r="F2">
+        <v>5</v>
+      </c>
+      <c r="G2">
+        <v>40</v>
+      </c>
+      <c r="H2">
+        <v>27</v>
+      </c>
+      <c r="I2">
+        <v>26</v>
+      </c>
+      <c r="J2">
+        <v>66</v>
+      </c>
+      <c r="K2">
+        <v>25</v>
+      </c>
+      <c r="L2">
+        <v>5</v>
+      </c>
+      <c r="M2">
+        <v>23</v>
+      </c>
+      <c r="N2">
+        <v>21</v>
+      </c>
+      <c r="O2">
+        <v>40</v>
+      </c>
+      <c r="P2">
+        <v>3</v>
+      </c>
+      <c r="Q2">
+        <v>5</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>6</v>
+      </c>
+      <c r="T2">
+        <v>16</v>
+      </c>
+      <c r="U2" s="1">
+        <f>6/103</f>
+        <v>5.8252427184466021E-2</v>
+      </c>
+      <c r="V2" s="1">
+        <f>43/103</f>
+        <v>0.41747572815533979</v>
+      </c>
+      <c r="W2" s="1">
+        <f>30/103</f>
+        <v>0.29126213592233008</v>
+      </c>
+      <c r="Z2" s="1">
+        <f>25/103</f>
+        <v>0.24271844660194175</v>
+      </c>
+      <c r="AA2" s="1">
+        <f>6/103</f>
+        <v>5.8252427184466021E-2</v>
+      </c>
+      <c r="AB2" s="1">
+        <f>25/103</f>
+        <v>0.24271844660194175</v>
+      </c>
+      <c r="AC2" s="1">
+        <f>23/103</f>
+        <v>0.22330097087378642</v>
+      </c>
+      <c r="AD2" s="1">
+        <f>42/103</f>
+        <v>0.40776699029126212</v>
+      </c>
+      <c r="AE2" s="1">
+        <f>3/103</f>
+        <v>2.9126213592233011E-2</v>
+      </c>
+      <c r="AF2" s="1">
+        <f>5/103</f>
+        <v>4.8543689320388349E-2</v>
+      </c>
+      <c r="AG2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AH2" s="1">
+        <f>6/103</f>
+        <v>5.8252427184466021E-2</v>
+      </c>
+      <c r="AI2" s="1">
+        <f>17/103</f>
+        <v>0.1650485436893204</v>
+      </c>
+    </row>
+    <row r="3" spans="2:35" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3">
+        <v>8</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
+      </c>
+      <c r="H3">
+        <v>3</v>
+      </c>
+      <c r="I3">
+        <v>3</v>
+      </c>
+      <c r="J3">
+        <v>5</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <v>2</v>
+      </c>
+      <c r="N3">
+        <v>2</v>
+      </c>
+      <c r="O3">
+        <v>2</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <v>1</v>
+      </c>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
+      <c r="W3" s="1"/>
+      <c r="Z3" s="1"/>
+      <c r="AA3" s="1"/>
+      <c r="AB3" s="1"/>
+      <c r="AC3" s="1"/>
+      <c r="AD3" s="1"/>
+      <c r="AE3" s="1"/>
+      <c r="AF3" s="1"/>
+      <c r="AG3" s="1"/>
+      <c r="AH3" s="1"/>
+      <c r="AI3" s="1"/>
+    </row>
+    <row r="4" spans="2:35" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4">
+        <v>326</v>
+      </c>
+      <c r="E4">
+        <v>384</v>
+      </c>
+      <c r="F4">
+        <v>40</v>
+      </c>
+      <c r="G4">
+        <v>153</v>
+      </c>
+      <c r="H4">
+        <v>71</v>
+      </c>
+      <c r="I4">
+        <v>73</v>
+      </c>
+      <c r="J4">
+        <v>244</v>
+      </c>
+      <c r="K4">
+        <v>86</v>
+      </c>
+      <c r="L4">
+        <v>25</v>
+      </c>
+      <c r="M4">
+        <v>65</v>
+      </c>
+      <c r="N4">
+        <v>88</v>
+      </c>
+      <c r="O4">
+        <v>182</v>
+      </c>
+      <c r="P4">
+        <v>8</v>
+      </c>
+      <c r="Q4">
+        <v>3</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>18</v>
+      </c>
+      <c r="T4">
+        <v>63</v>
+      </c>
+      <c r="U4" s="1">
+        <f>44/392</f>
+        <v>0.11224489795918367</v>
+      </c>
+      <c r="V4" s="1">
+        <f>177/392</f>
+        <v>0.45153061224489793</v>
+      </c>
+      <c r="W4" s="1">
+        <f>87/392</f>
+        <v>0.22193877551020408</v>
+      </c>
+      <c r="Z4" s="1">
+        <f>102/392</f>
+        <v>0.26020408163265307</v>
+      </c>
+      <c r="AA4" s="1">
+        <f>30/392</f>
+        <v>7.6530612244897961E-2</v>
+      </c>
+      <c r="AB4" s="1">
+        <f>81/392</f>
+        <v>0.2066326530612245</v>
+      </c>
+      <c r="AC4" s="1">
+        <f>109/392</f>
+        <v>0.27806122448979592</v>
+      </c>
+      <c r="AD4" s="1">
+        <f>198/392</f>
+        <v>0.50510204081632648</v>
+      </c>
+      <c r="AE4" s="1">
+        <f>10/392</f>
+        <v>2.5510204081632654E-2</v>
+      </c>
+      <c r="AF4" s="1">
+        <f>5/392</f>
+        <v>1.2755102040816327E-2</v>
+      </c>
+      <c r="AG4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AH4" s="1">
+        <f>26/392</f>
+        <v>6.6326530612244902E-2</v>
+      </c>
+      <c r="AI4" s="1">
+        <f>74/392</f>
+        <v>0.18877551020408162</v>
+      </c>
+    </row>
+    <row r="5" spans="2:35" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5">
+        <v>58</v>
+      </c>
+      <c r="F5">
+        <v>4</v>
+      </c>
+      <c r="G5">
+        <v>24</v>
+      </c>
+      <c r="H5">
+        <v>16</v>
+      </c>
+      <c r="I5">
+        <v>20</v>
+      </c>
+      <c r="J5">
+        <v>38</v>
+      </c>
+      <c r="K5">
+        <v>16</v>
+      </c>
+      <c r="L5">
+        <v>5</v>
+      </c>
+      <c r="M5">
+        <v>16</v>
+      </c>
+      <c r="N5">
+        <v>21</v>
+      </c>
+      <c r="O5">
+        <v>16</v>
+      </c>
+      <c r="P5">
+        <v>2</v>
+      </c>
+      <c r="Q5">
+        <v>2</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>8</v>
+      </c>
+      <c r="T5">
+        <v>11</v>
+      </c>
+      <c r="U5" s="1"/>
+      <c r="V5" s="1"/>
+      <c r="W5" s="1"/>
+      <c r="Z5" s="1"/>
+      <c r="AA5" s="1"/>
+      <c r="AB5" s="1"/>
+      <c r="AC5" s="1"/>
+      <c r="AD5" s="1"/>
+      <c r="AE5" s="1"/>
+      <c r="AF5" s="1"/>
+      <c r="AG5" s="1"/>
+      <c r="AH5" s="1"/>
+      <c r="AI5" s="1"/>
+    </row>
+    <row r="6" spans="2:35" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6">
+        <v>2121</v>
+      </c>
+      <c r="E6">
+        <v>2376</v>
+      </c>
+      <c r="F6">
+        <v>106</v>
+      </c>
+      <c r="G6">
+        <v>1066</v>
+      </c>
+      <c r="H6">
+        <v>465</v>
+      </c>
+      <c r="I6">
+        <v>561</v>
+      </c>
+      <c r="J6">
+        <v>1529</v>
+      </c>
+      <c r="K6">
+        <v>510</v>
+      </c>
+      <c r="L6">
+        <v>195</v>
+      </c>
+      <c r="M6">
+        <v>456</v>
+      </c>
+      <c r="N6">
+        <v>523</v>
+      </c>
+      <c r="O6">
+        <v>1046</v>
+      </c>
+      <c r="P6">
+        <v>65</v>
+      </c>
+      <c r="Q6">
+        <v>31</v>
+      </c>
+      <c r="R6">
+        <v>1</v>
+      </c>
+      <c r="S6">
+        <v>105</v>
+      </c>
+      <c r="T6">
+        <v>286</v>
+      </c>
+      <c r="U6" s="1">
+        <f>121/2468</f>
+        <v>4.9027552674230146E-2</v>
+      </c>
+      <c r="V6" s="1">
+        <f>1180/2468</f>
+        <v>0.47811993517017826</v>
+      </c>
+      <c r="W6" s="1">
+        <f>526/2468</f>
+        <v>0.21312803889789303</v>
+      </c>
+      <c r="Z6" s="1">
+        <f>574/2468</f>
+        <v>0.23257698541329011</v>
+      </c>
+      <c r="AA6" s="1">
+        <f>225/2468</f>
+        <v>9.116693679092383E-2</v>
+      </c>
+      <c r="AB6" s="1">
+        <f>521/2468</f>
+        <v>0.21110210696920584</v>
+      </c>
+      <c r="AC6" s="1">
+        <f>592/2468</f>
+        <v>0.23987034035656402</v>
+      </c>
+      <c r="AD6" s="1">
+        <f>1144/2468</f>
+        <v>0.46353322528363045</v>
+      </c>
+      <c r="AE6" s="1">
+        <f>77/2468</f>
+        <v>3.119935170178282E-2</v>
+      </c>
+      <c r="AF6" s="1">
+        <f>34/2468</f>
+        <v>1.3776337115072933E-2</v>
+      </c>
+      <c r="AG6" s="1">
+        <f>1/2468</f>
+        <v>4.051863857374392E-4</v>
+      </c>
+      <c r="AH6" s="1">
+        <f>116/2468</f>
+        <v>4.7001620745542948E-2</v>
+      </c>
+      <c r="AI6" s="1">
+        <f>330/2468</f>
+        <v>0.13371150729335493</v>
+      </c>
+    </row>
+    <row r="7" spans="2:35" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7">
+        <v>255</v>
+      </c>
+      <c r="F7">
+        <v>15</v>
+      </c>
+      <c r="G7">
+        <v>114</v>
+      </c>
+      <c r="H7">
+        <v>61</v>
+      </c>
+      <c r="I7">
+        <v>95</v>
+      </c>
+      <c r="J7">
+        <v>157</v>
+      </c>
+      <c r="K7">
+        <v>64</v>
+      </c>
+      <c r="L7">
+        <v>30</v>
+      </c>
+      <c r="M7">
+        <v>65</v>
+      </c>
+      <c r="N7">
+        <v>69</v>
+      </c>
+      <c r="O7">
+        <v>98</v>
+      </c>
+      <c r="P7">
+        <v>12</v>
+      </c>
+      <c r="Q7">
+        <v>3</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <v>11</v>
+      </c>
+      <c r="T7">
+        <v>44</v>
+      </c>
+      <c r="U7" s="1"/>
+      <c r="V7" s="1"/>
+      <c r="W7" s="1"/>
+      <c r="Z7" s="1"/>
+      <c r="AA7" s="1"/>
+      <c r="AB7" s="1"/>
+      <c r="AC7" s="1"/>
+      <c r="AD7" s="1"/>
+      <c r="AE7" s="1"/>
+      <c r="AF7" s="1"/>
+      <c r="AG7" s="1"/>
+      <c r="AH7" s="1"/>
+      <c r="AI7" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Verified accuracy of final sum numbers
</commit_message>
<xml_diff>
--- a/Resources/Compiled.xlsx
+++ b/Resources/Compiled.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tyleah1/Desktop/nyc_squirrels/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{591D1D2A-67C9-FB4B-AC22-50D25162F1F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{718ACD48-5C83-E044-806B-45CD39AC8086}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3760" yWindow="460" windowWidth="21720" windowHeight="16960" xr2:uid="{2CC0A3FC-6AB6-1249-9AAB-1F178B143B2D}"/>
   </bookViews>
@@ -519,7 +519,7 @@
   <dimension ref="B1:AI7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="AC11" sqref="AC11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -698,44 +698,52 @@
         <f>30/103</f>
         <v>0.29126213592233008</v>
       </c>
+      <c r="X2" s="1">
+        <f>29/100</f>
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="Y2" s="1">
+        <f>71/100</f>
+        <v>0.71</v>
+      </c>
       <c r="Z2" s="1">
-        <f>25/103</f>
-        <v>0.24271844660194175</v>
+        <f>25/100</f>
+        <v>0.25</v>
       </c>
       <c r="AA2" s="1">
-        <f>6/103</f>
-        <v>5.8252427184466021E-2</v>
+        <f>6/100</f>
+        <v>0.06</v>
       </c>
       <c r="AB2" s="1">
-        <f>25/103</f>
-        <v>0.24271844660194175</v>
+        <f>25/100</f>
+        <v>0.25</v>
       </c>
       <c r="AC2" s="1">
-        <f>23/103</f>
-        <v>0.22330097087378642</v>
+        <f>23/100</f>
+        <v>0.23</v>
       </c>
       <c r="AD2" s="1">
-        <f>42/103</f>
-        <v>0.40776699029126212</v>
+        <f>42/100</f>
+        <v>0.42</v>
       </c>
       <c r="AE2" s="1">
-        <f>3/103</f>
-        <v>2.9126213592233011E-2</v>
+        <f>3/100</f>
+        <v>0.03</v>
       </c>
       <c r="AF2" s="1">
-        <f>5/103</f>
-        <v>4.8543689320388349E-2</v>
+        <f>5/100</f>
+        <v>0.05</v>
       </c>
       <c r="AG2" s="1">
         <v>0</v>
       </c>
       <c r="AH2" s="1">
-        <f>6/103</f>
-        <v>5.8252427184466021E-2</v>
+        <f>6/100</f>
+        <v>0.06</v>
       </c>
       <c r="AI2" s="1">
-        <f>17/103</f>
-        <v>0.1650485436893204</v>
+        <f>17/100</f>
+        <v>0.17</v>
       </c>
     </row>
     <row r="3" spans="2:35" x14ac:dyDescent="0.2">
@@ -796,6 +804,8 @@
       <c r="U3" s="1"/>
       <c r="V3" s="1"/>
       <c r="W3" s="1"/>
+      <c r="X3" s="1"/>
+      <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
       <c r="AA3" s="1"/>
       <c r="AB3" s="1"/>
@@ -877,44 +887,52 @@
         <f>87/392</f>
         <v>0.22193877551020408</v>
       </c>
+      <c r="X4" s="1">
+        <f>93/384</f>
+        <v>0.2421875</v>
+      </c>
+      <c r="Y4" s="1">
+        <f>282/384</f>
+        <v>0.734375</v>
+      </c>
       <c r="Z4" s="1">
-        <f>102/392</f>
-        <v>0.26020408163265307</v>
+        <f>102/384</f>
+        <v>0.265625</v>
       </c>
       <c r="AA4" s="1">
-        <f>30/392</f>
-        <v>7.6530612244897961E-2</v>
+        <f>30/384</f>
+        <v>7.8125E-2</v>
       </c>
       <c r="AB4" s="1">
-        <f>81/392</f>
-        <v>0.2066326530612245</v>
+        <f>81/384</f>
+        <v>0.2109375</v>
       </c>
       <c r="AC4" s="1">
-        <f>109/392</f>
-        <v>0.27806122448979592</v>
+        <f>109/384</f>
+        <v>0.28385416666666669</v>
       </c>
       <c r="AD4" s="1">
-        <f>198/392</f>
-        <v>0.50510204081632648</v>
+        <f>198/384</f>
+        <v>0.515625</v>
       </c>
       <c r="AE4" s="1">
-        <f>10/392</f>
-        <v>2.5510204081632654E-2</v>
+        <f>10/384</f>
+        <v>2.6041666666666668E-2</v>
       </c>
       <c r="AF4" s="1">
-        <f>5/392</f>
-        <v>1.2755102040816327E-2</v>
+        <f>5/384</f>
+        <v>1.3020833333333334E-2</v>
       </c>
       <c r="AG4" s="1">
         <v>0</v>
       </c>
       <c r="AH4" s="1">
-        <f>26/392</f>
-        <v>6.6326530612244902E-2</v>
+        <f>26/384</f>
+        <v>6.7708333333333329E-2</v>
       </c>
       <c r="AI4" s="1">
-        <f>74/392</f>
-        <v>0.18877551020408162</v>
+        <f>74/384</f>
+        <v>0.19270833333333334</v>
       </c>
     </row>
     <row r="5" spans="2:35" x14ac:dyDescent="0.2">
@@ -975,6 +993,8 @@
       <c r="U5" s="1"/>
       <c r="V5" s="1"/>
       <c r="W5" s="1"/>
+      <c r="X5" s="1"/>
+      <c r="Y5" s="1"/>
       <c r="Z5" s="1"/>
       <c r="AA5" s="1"/>
       <c r="AB5" s="1"/>
@@ -1056,45 +1076,53 @@
         <f>526/2468</f>
         <v>0.21312803889789303</v>
       </c>
+      <c r="X6" s="1">
+        <f>656/2376</f>
+        <v>0.27609427609427611</v>
+      </c>
+      <c r="Y6" s="1">
+        <f>1686/2376</f>
+        <v>0.70959595959595956</v>
+      </c>
       <c r="Z6" s="1">
-        <f>574/2468</f>
-        <v>0.23257698541329011</v>
+        <f>574/2376</f>
+        <v>0.24158249158249159</v>
       </c>
       <c r="AA6" s="1">
-        <f>225/2468</f>
-        <v>9.116693679092383E-2</v>
+        <f>225/2376</f>
+        <v>9.4696969696969696E-2</v>
       </c>
       <c r="AB6" s="1">
-        <f>521/2468</f>
-        <v>0.21110210696920584</v>
+        <f>521/2376</f>
+        <v>0.21927609427609426</v>
       </c>
       <c r="AC6" s="1">
-        <f>592/2468</f>
-        <v>0.23987034035656402</v>
+        <f>592/2376</f>
+        <v>0.24915824915824916</v>
       </c>
       <c r="AD6" s="1">
-        <f>1144/2468</f>
-        <v>0.46353322528363045</v>
+        <f>1144/2376</f>
+        <v>0.48148148148148145</v>
       </c>
       <c r="AE6" s="1">
-        <f>77/2468</f>
-        <v>3.119935170178282E-2</v>
+        <f>77/2376</f>
+        <v>3.2407407407407406E-2</v>
       </c>
       <c r="AF6" s="1">
-        <f>34/2468</f>
-        <v>1.3776337115072933E-2</v>
+        <f>34/2376</f>
+        <v>1.4309764309764311E-2</v>
       </c>
       <c r="AG6" s="1">
-        <f>1/2468</f>
-        <v>4.051863857374392E-4</v>
+        <f>1/2376</f>
+        <v>4.2087542087542086E-4</v>
       </c>
       <c r="AH6" s="1">
-        <f>116/2468</f>
-        <v>4.7001620745542948E-2</v>
+        <f>116/2376</f>
+        <v>4.8821548821548821E-2</v>
       </c>
       <c r="AI6" s="1">
-        <f>330/2468</f>
-        <v>0.13371150729335493</v>
+        <f>330/2376</f>
+        <v>0.1388888888888889</v>
       </c>
     </row>
     <row r="7" spans="2:35" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Updated images for report
</commit_message>
<xml_diff>
--- a/Resources/Compiled.xlsx
+++ b/Resources/Compiled.xlsx
@@ -8,12 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tyleah1/Desktop/nyc_squirrels/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{718ACD48-5C83-E044-806B-45CD39AC8086}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BE04875-6F73-CC4E-8D3F-3A7F376FF07F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3760" yWindow="460" windowWidth="21720" windowHeight="16960" xr2:uid="{2CC0A3FC-6AB6-1249-9AAB-1F178B143B2D}"/>
+    <workbookView xWindow="60" yWindow="460" windowWidth="26400" windowHeight="16960" activeTab="3" xr2:uid="{2CC0A3FC-6AB6-1249-9AAB-1F178B143B2D}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Age Separated" sheetId="1" r:id="rId1"/>
+    <sheet name="Combined" sheetId="2" r:id="rId2"/>
+    <sheet name="Transposed" sheetId="4" r:id="rId3"/>
+    <sheet name="Groups" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="52">
   <si>
     <t>age</t>
   </si>
@@ -152,6 +155,45 @@
   </si>
   <si>
     <t>Total_age</t>
+  </si>
+  <si>
+    <t>approach</t>
+  </si>
+  <si>
+    <t>on_ground</t>
+  </si>
+  <si>
+    <t>tail_twich</t>
+  </si>
+  <si>
+    <t>run</t>
+  </si>
+  <si>
+    <t>chase</t>
+  </si>
+  <si>
+    <t>climb</t>
+  </si>
+  <si>
+    <t>eat</t>
+  </si>
+  <si>
+    <t>forage</t>
+  </si>
+  <si>
+    <t>Set</t>
+  </si>
+  <si>
+    <t>Communication</t>
+  </si>
+  <si>
+    <t>Activities</t>
+  </si>
+  <si>
+    <t>Interactions</t>
+  </si>
+  <si>
+    <t>Locations</t>
   </si>
 </sst>
 </file>
@@ -159,9 +201,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -172,6 +214,13 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -198,9 +247,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -516,10 +568,280 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99D8C755-B0EB-9540-A1B2-9FD485A6C973}">
+  <dimension ref="A1:Q4"/>
+  <sheetViews>
+    <sheetView zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:L2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L1" t="s">
+        <v>46</v>
+      </c>
+      <c r="M1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O1" t="s">
+        <v>8</v>
+      </c>
+      <c r="P1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="1">
+        <f>6/103</f>
+        <v>5.8252427184466021E-2</v>
+      </c>
+      <c r="D2" s="1">
+        <f>43/103</f>
+        <v>0.41747572815533979</v>
+      </c>
+      <c r="E2" s="1">
+        <f>30/103</f>
+        <v>0.29126213592233008</v>
+      </c>
+      <c r="F2" s="1">
+        <f>29/100</f>
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="G2" s="1">
+        <f>71/100</f>
+        <v>0.71</v>
+      </c>
+      <c r="H2" s="1">
+        <f>25/100</f>
+        <v>0.25</v>
+      </c>
+      <c r="I2" s="1">
+        <f>6/100</f>
+        <v>0.06</v>
+      </c>
+      <c r="J2" s="1">
+        <f>25/100</f>
+        <v>0.25</v>
+      </c>
+      <c r="K2" s="1">
+        <f>23/100</f>
+        <v>0.23</v>
+      </c>
+      <c r="L2" s="1">
+        <f>42/100</f>
+        <v>0.42</v>
+      </c>
+      <c r="M2" s="1">
+        <f>3/100</f>
+        <v>0.03</v>
+      </c>
+      <c r="N2" s="1">
+        <f>5/100</f>
+        <v>0.05</v>
+      </c>
+      <c r="O2" s="1">
+        <v>0</v>
+      </c>
+      <c r="P2" s="1">
+        <f>6/100</f>
+        <v>0.06</v>
+      </c>
+      <c r="Q2" s="1">
+        <f>17/100</f>
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="1">
+        <f>44/392</f>
+        <v>0.11224489795918367</v>
+      </c>
+      <c r="D3" s="1">
+        <f>177/392</f>
+        <v>0.45153061224489793</v>
+      </c>
+      <c r="E3" s="1">
+        <f>87/392</f>
+        <v>0.22193877551020408</v>
+      </c>
+      <c r="F3" s="1">
+        <f>93/384</f>
+        <v>0.2421875</v>
+      </c>
+      <c r="G3" s="1">
+        <f>282/384</f>
+        <v>0.734375</v>
+      </c>
+      <c r="H3" s="1">
+        <f>102/384</f>
+        <v>0.265625</v>
+      </c>
+      <c r="I3" s="1">
+        <f>30/384</f>
+        <v>7.8125E-2</v>
+      </c>
+      <c r="J3" s="1">
+        <f>81/384</f>
+        <v>0.2109375</v>
+      </c>
+      <c r="K3" s="1">
+        <f>109/384</f>
+        <v>0.28385416666666669</v>
+      </c>
+      <c r="L3" s="1">
+        <f>198/384</f>
+        <v>0.515625</v>
+      </c>
+      <c r="M3" s="1">
+        <f>10/384</f>
+        <v>2.6041666666666668E-2</v>
+      </c>
+      <c r="N3" s="1">
+        <f>5/384</f>
+        <v>1.3020833333333334E-2</v>
+      </c>
+      <c r="O3" s="1">
+        <v>0</v>
+      </c>
+      <c r="P3" s="1">
+        <f>26/384</f>
+        <v>6.7708333333333329E-2</v>
+      </c>
+      <c r="Q3" s="1">
+        <f>74/384</f>
+        <v>0.19270833333333334</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="1">
+        <f>121/2468</f>
+        <v>4.9027552674230146E-2</v>
+      </c>
+      <c r="D4" s="1">
+        <f>1180/2468</f>
+        <v>0.47811993517017826</v>
+      </c>
+      <c r="E4" s="1">
+        <f>526/2468</f>
+        <v>0.21312803889789303</v>
+      </c>
+      <c r="F4" s="1">
+        <f>656/2376</f>
+        <v>0.27609427609427611</v>
+      </c>
+      <c r="G4" s="1">
+        <f>1686/2376</f>
+        <v>0.70959595959595956</v>
+      </c>
+      <c r="H4" s="1">
+        <f>574/2376</f>
+        <v>0.24158249158249159</v>
+      </c>
+      <c r="I4" s="1">
+        <f>225/2376</f>
+        <v>9.4696969696969696E-2</v>
+      </c>
+      <c r="J4" s="1">
+        <f>521/2376</f>
+        <v>0.21927609427609426</v>
+      </c>
+      <c r="K4" s="1">
+        <f>592/2376</f>
+        <v>0.24915824915824916</v>
+      </c>
+      <c r="L4" s="1">
+        <f>1144/2376</f>
+        <v>0.48148148148148145</v>
+      </c>
+      <c r="M4" s="1">
+        <f>77/2376</f>
+        <v>3.2407407407407406E-2</v>
+      </c>
+      <c r="N4" s="1">
+        <f>34/2376</f>
+        <v>1.4309764309764311E-2</v>
+      </c>
+      <c r="O4" s="1">
+        <f>1/2376</f>
+        <v>4.2087542087542086E-4</v>
+      </c>
+      <c r="P4" s="1">
+        <f>116/2376</f>
+        <v>4.8821548821548821E-2</v>
+      </c>
+      <c r="Q4" s="1">
+        <f>330/2376</f>
+        <v>0.1388888888888889</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{442C2500-6E68-7245-BB3C-9BFFFD01A0D6}">
   <dimension ref="B1:AI7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <selection activeCell="AC11" sqref="AC11"/>
+    <sheetView topLeftCell="G1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1197,4 +1519,691 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BA07A1D-96CC-D547-BB21-75F64E5BEA17}">
+  <dimension ref="A1:D16"/>
+  <sheetViews>
+    <sheetView zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="2">
+        <f>6/103</f>
+        <v>5.8252427184466021E-2</v>
+      </c>
+      <c r="C2" s="2">
+        <f>44/392</f>
+        <v>0.11224489795918367</v>
+      </c>
+      <c r="D2" s="2">
+        <f>121/2468</f>
+        <v>4.9027552674230146E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="2">
+        <f>43/103</f>
+        <v>0.41747572815533979</v>
+      </c>
+      <c r="C3" s="2">
+        <f>177/392</f>
+        <v>0.45153061224489793</v>
+      </c>
+      <c r="D3" s="2">
+        <f>1180/2468</f>
+        <v>0.47811993517017826</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="2">
+        <f>30/103</f>
+        <v>0.29126213592233008</v>
+      </c>
+      <c r="C4" s="2">
+        <f>87/392</f>
+        <v>0.22193877551020408</v>
+      </c>
+      <c r="D4" s="2">
+        <f>526/2468</f>
+        <v>0.21312803889789303</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="2">
+        <f>29/100</f>
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="C5" s="2">
+        <f>93/384</f>
+        <v>0.2421875</v>
+      </c>
+      <c r="D5" s="2">
+        <f>656/2376</f>
+        <v>0.27609427609427611</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="2">
+        <f>71/100</f>
+        <v>0.71</v>
+      </c>
+      <c r="C6" s="2">
+        <f>282/384</f>
+        <v>0.734375</v>
+      </c>
+      <c r="D6" s="2">
+        <f>1686/2376</f>
+        <v>0.70959595959595956</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="2">
+        <f>25/100</f>
+        <v>0.25</v>
+      </c>
+      <c r="C7" s="2">
+        <f>102/384</f>
+        <v>0.265625</v>
+      </c>
+      <c r="D7" s="2">
+        <f>574/2376</f>
+        <v>0.24158249158249159</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="2">
+        <f>6/100</f>
+        <v>0.06</v>
+      </c>
+      <c r="C8" s="2">
+        <f>30/384</f>
+        <v>7.8125E-2</v>
+      </c>
+      <c r="D8" s="2">
+        <f>225/2376</f>
+        <v>9.4696969696969696E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="2">
+        <f>25/100</f>
+        <v>0.25</v>
+      </c>
+      <c r="C9" s="2">
+        <f>81/384</f>
+        <v>0.2109375</v>
+      </c>
+      <c r="D9" s="2">
+        <f>521/2376</f>
+        <v>0.21927609427609426</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="2">
+        <f>23/100</f>
+        <v>0.23</v>
+      </c>
+      <c r="C10" s="2">
+        <f>109/384</f>
+        <v>0.28385416666666669</v>
+      </c>
+      <c r="D10" s="2">
+        <f>592/2376</f>
+        <v>0.24915824915824916</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="2">
+        <f>42/100</f>
+        <v>0.42</v>
+      </c>
+      <c r="C11" s="2">
+        <f>198/384</f>
+        <v>0.515625</v>
+      </c>
+      <c r="D11" s="2">
+        <f>1144/2376</f>
+        <v>0.48148148148148145</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="2">
+        <f>3/100</f>
+        <v>0.03</v>
+      </c>
+      <c r="C12" s="2">
+        <f>10/384</f>
+        <v>2.6041666666666668E-2</v>
+      </c>
+      <c r="D12" s="2">
+        <f>77/2376</f>
+        <v>3.2407407407407406E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="2">
+        <f>5/100</f>
+        <v>0.05</v>
+      </c>
+      <c r="C13" s="2">
+        <f>5/384</f>
+        <v>1.3020833333333334E-2</v>
+      </c>
+      <c r="D13" s="2">
+        <f>34/2376</f>
+        <v>1.4309764309764311E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="3">
+        <v>0</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0</v>
+      </c>
+      <c r="D14" s="3">
+        <f>1/2376</f>
+        <v>4.2087542087542086E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="2">
+        <f>6/100</f>
+        <v>0.06</v>
+      </c>
+      <c r="C15" s="2">
+        <f>26/384</f>
+        <v>6.7708333333333329E-2</v>
+      </c>
+      <c r="D15" s="2">
+        <f>116/2376</f>
+        <v>4.8821548821548821E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" s="2">
+        <f>17/100</f>
+        <v>0.17</v>
+      </c>
+      <c r="C16" s="2">
+        <f>74/384</f>
+        <v>0.19270833333333334</v>
+      </c>
+      <c r="D16" s="2">
+        <f>330/2376</f>
+        <v>0.1388888888888889</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28B78B8F-6378-6B49-B7EC-CF53C326DA9C}">
+  <dimension ref="A1:Q13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1">
+        <f>3/100</f>
+        <v>0.03</v>
+      </c>
+      <c r="N2" s="1">
+        <f>5/100</f>
+        <v>0.05</v>
+      </c>
+      <c r="O2" s="1">
+        <v>0</v>
+      </c>
+      <c r="P2" s="1">
+        <f>6/100</f>
+        <v>0.06</v>
+      </c>
+      <c r="Q2" s="1">
+        <f>17/100</f>
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1">
+        <f>25/100</f>
+        <v>0.25</v>
+      </c>
+      <c r="I3" s="1">
+        <f>6/100</f>
+        <v>0.06</v>
+      </c>
+      <c r="J3" s="1">
+        <f>25/100</f>
+        <v>0.25</v>
+      </c>
+      <c r="K3" s="1">
+        <f>23/100</f>
+        <v>0.23</v>
+      </c>
+      <c r="L3" s="1">
+        <f>42/100</f>
+        <v>0.42</v>
+      </c>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="1">
+        <f>6/103</f>
+        <v>5.8252427184466021E-2</v>
+      </c>
+      <c r="D4" s="1">
+        <f>43/103</f>
+        <v>0.41747572815533979</v>
+      </c>
+      <c r="E4" s="1">
+        <f>30/103</f>
+        <v>0.29126213592233008</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="1">
+        <f>29/100</f>
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="G5" s="1">
+        <f>71/100</f>
+        <v>0.71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="M6" s="1">
+        <f>10/384</f>
+        <v>2.6041666666666668E-2</v>
+      </c>
+      <c r="N6" s="1">
+        <f>5/384</f>
+        <v>1.3020833333333334E-2</v>
+      </c>
+      <c r="O6" s="1">
+        <v>0</v>
+      </c>
+      <c r="P6" s="1">
+        <f>26/384</f>
+        <v>6.7708333333333329E-2</v>
+      </c>
+      <c r="Q6" s="1">
+        <f>74/384</f>
+        <v>0.19270833333333334</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" s="1">
+        <f>102/384</f>
+        <v>0.265625</v>
+      </c>
+      <c r="I7" s="1">
+        <f>30/384</f>
+        <v>7.8125E-2</v>
+      </c>
+      <c r="J7" s="1">
+        <f>81/384</f>
+        <v>0.2109375</v>
+      </c>
+      <c r="K7" s="1">
+        <f>109/384</f>
+        <v>0.28385416666666669</v>
+      </c>
+      <c r="L7" s="1">
+        <f>198/384</f>
+        <v>0.515625</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="1">
+        <f>44/392</f>
+        <v>0.11224489795918367</v>
+      </c>
+      <c r="D8" s="1">
+        <f>177/392</f>
+        <v>0.45153061224489793</v>
+      </c>
+      <c r="E8" s="1">
+        <f>87/392</f>
+        <v>0.22193877551020408</v>
+      </c>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1">
+        <f>93/384</f>
+        <v>0.2421875</v>
+      </c>
+      <c r="G9" s="1">
+        <f>282/384</f>
+        <v>0.734375</v>
+      </c>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="M10" s="1">
+        <f>77/2376</f>
+        <v>3.2407407407407406E-2</v>
+      </c>
+      <c r="N10" s="1">
+        <f>34/2376</f>
+        <v>1.4309764309764311E-2</v>
+      </c>
+      <c r="O10" s="1">
+        <f>1/2376</f>
+        <v>4.2087542087542086E-4</v>
+      </c>
+      <c r="P10" s="1">
+        <f>116/2376</f>
+        <v>4.8821548821548821E-2</v>
+      </c>
+      <c r="Q10" s="1">
+        <f>330/2376</f>
+        <v>0.1388888888888889</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H11" s="1">
+        <f>574/2376</f>
+        <v>0.24158249158249159</v>
+      </c>
+      <c r="I11" s="1">
+        <f>225/2376</f>
+        <v>9.4696969696969696E-2</v>
+      </c>
+      <c r="J11" s="1">
+        <f>521/2376</f>
+        <v>0.21927609427609426</v>
+      </c>
+      <c r="K11" s="1">
+        <f>592/2376</f>
+        <v>0.24915824915824916</v>
+      </c>
+      <c r="L11" s="1">
+        <f>1144/2376</f>
+        <v>0.48148148148148145</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="1">
+        <f>121/2468</f>
+        <v>4.9027552674230146E-2</v>
+      </c>
+      <c r="D12" s="1">
+        <f>1180/2468</f>
+        <v>0.47811993517017826</v>
+      </c>
+      <c r="E12" s="1">
+        <f>526/2468</f>
+        <v>0.21312803889789303</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" s="1">
+        <f>656/2376</f>
+        <v>0.27609427609427611</v>
+      </c>
+      <c r="G13" s="1">
+        <f>1686/2376</f>
+        <v>0.70959595959595956</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>